<commit_message>
Update Sequence Diagram + Add Manage Homepage Sequence
</commit_message>
<xml_diff>
--- a/1.DELIVERABLE/1.7 PROCESS/BSS_RiskList_V1.0.xlsx
+++ b/1.DELIVERABLE/1.7 PROCESS/BSS_RiskList_V1.0.xlsx
@@ -120,7 +120,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFF3333"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,63 +452,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -526,6 +526,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3333"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -824,7 +829,7 @@
   <dimension ref="C1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -838,15 +843,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:12" ht="37.5" x14ac:dyDescent="0.5">
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D2" s="2"/>
@@ -876,48 +881,48 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
       <c r="J4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="3:12" s="3" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="C5" s="11"/>
       <c r="D5" s="7">
         <v>2</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="3:12" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="D6" s="7">
         <v>3</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="28"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5" t="s">
         <v>10</v>
       </c>
@@ -928,69 +933,69 @@
       <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
       <c r="J7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="3:12" ht="37.5" x14ac:dyDescent="0.3">
       <c r="D8" s="7">
         <v>5</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D9" s="7">
         <v>6</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
       <c r="J9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D10" s="8">
         <v>7</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
       <c r="J10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D11" s="17"/>

</xml_diff>